<commit_message>
:beers: I slowly continue
</commit_message>
<xml_diff>
--- a/Matrix.xlsx
+++ b/Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\DataGripProjects\dbsec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\DataGripProjects\db-security-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBA93F3-0199-48E5-8A52-0475BB2EC08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44633F7-3100-4D8D-9EB2-37D5ADB9D75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6550" yWindow="8690" windowWidth="28800" windowHeight="15410" xr2:uid="{FB151949-07DF-9E4B-ADDA-32C56BC4D90F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{FB151949-07DF-9E4B-ADDA-32C56BC4D90F}"/>
   </bookViews>
   <sheets>
     <sheet name="Process-user matrix" sheetId="1" r:id="rId1"/>
@@ -38,14 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="57">
   <si>
     <t>Process-user matrix</t>
   </si>
   <si>
-    <t>Administrators</t>
-  </si>
-  <si>
     <t>Employees</t>
   </si>
   <si>
@@ -76,9 +73,6 @@
     <t>Pay invoice</t>
   </si>
   <si>
-    <t>Send invoice</t>
-  </si>
-  <si>
     <t>View invoice</t>
   </si>
   <si>
@@ -154,9 +148,6 @@
     <t>Employee</t>
   </si>
   <si>
-    <t>Models_equipements_pricings</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -166,9 +157,6 @@
     <t>I,U,D</t>
   </si>
   <si>
-    <t>U</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -181,34 +169,46 @@
     <t>Entity-user matrix</t>
   </si>
   <si>
-    <t>employee</t>
-  </si>
-  <si>
     <t>Fleet responsible</t>
   </si>
   <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>I,U,D,S</t>
-  </si>
-  <si>
-    <t>S,I,U,D</t>
-  </si>
-  <si>
-    <t>I,S,U</t>
-  </si>
-  <si>
-    <t>S,U,D,I</t>
-  </si>
-  <si>
-    <t>S,I,U</t>
-  </si>
-  <si>
     <t>Pricings</t>
   </si>
   <si>
-    <t>admin app</t>
+    <t>HR manager</t>
+  </si>
+  <si>
+    <t>Fleet reesponsible</t>
+  </si>
+  <si>
+    <t>Application administrator</t>
+  </si>
+  <si>
+    <t>Manage employees</t>
+  </si>
+  <si>
+    <t>The fleet responsible use a procedure to cancel a vehicle reservation if he put a vehicle as damaged</t>
+  </si>
+  <si>
+    <t>For scalability reason customers are users at application level</t>
+  </si>
+  <si>
+    <t>Customers are not DB users, they are users at the application level</t>
+  </si>
+  <si>
+    <t>U,S</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Admin app</t>
+  </si>
+  <si>
+    <t>S,I</t>
+  </si>
+  <si>
+    <t>Admin can also manage the list of states</t>
   </si>
 </sst>
 </file>
@@ -361,8 +361,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD3C6F1B-018A-814A-BAB2-8F3FAE647CD3}" name="Tableau1" displayName="Tableau1" ref="B3:L6" totalsRowShown="0">
-  <autoFilter ref="B3:L6" xr:uid="{AD3C6F1B-018A-814A-BAB2-8F3FAE647CD3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD3C6F1B-018A-814A-BAB2-8F3FAE647CD3}" name="Tableau1" displayName="Tableau1" ref="B3:L8" totalsRowShown="0">
+  <autoFilter ref="B3:L8" xr:uid="{AD3C6F1B-018A-814A-BAB2-8F3FAE647CD3}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{6E0619E5-D273-D74D-AF9D-840719E1F688}" name="Process-user matrix"/>
     <tableColumn id="2" xr3:uid="{73682482-EF9F-2B41-B13A-604249596F4B}" name="P1"/>
@@ -381,19 +381,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B015FF1E-8112-144D-9160-BE4EACC1C4EF}" name="Tableau367" displayName="Tableau367" ref="B19:C29" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="B19:C29" xr:uid="{B015FF1E-8112-144D-9160-BE4EACC1C4EF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{285ED5D0-9C49-48D1-B580-D390634D232F}" name="Tableau363" displayName="Tableau363" ref="B15:C25" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="B15:C25" xr:uid="{285ED5D0-9C49-48D1-B580-D390634D232F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3ACF7604-C71C-4142-A8AA-4ABADFDECA62}" name="ID" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{3F629260-FC3B-8944-92DF-D600AE0C7753}" name="Process"/>
+    <tableColumn id="1" xr3:uid="{35459B5A-4B3E-4530-8321-9B450516126A}" name="ID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{A5DE6B87-05C4-4E7F-8554-0EB8B0B8AB38}" name="Process"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B43A4B11-A654-8342-87E0-FF434B9827DC}" name="Tableau15" displayName="Tableau15" ref="B4:L17" totalsRowShown="0">
-  <autoFilter ref="B4:L17" xr:uid="{B43A4B11-A654-8342-87E0-FF434B9827DC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B43A4B11-A654-8342-87E0-FF434B9827DC}" name="Tableau15" displayName="Tableau15" ref="B4:L16" totalsRowShown="0">
+  <autoFilter ref="B4:L16" xr:uid="{B43A4B11-A654-8342-87E0-FF434B9827DC}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{4FAFE25D-D33B-BB45-B051-60611B74A325}" name="Entity-process matrix"/>
     <tableColumn id="2" xr3:uid="{B43170F5-2DC5-AD4D-8F11-C5EDFA8381E4}" name="P1"/>
@@ -412,8 +412,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0141266D-28EC-E044-97D4-AA3617150640}" name="Tableau36" displayName="Tableau36" ref="C25:D35" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="C25:D35" xr:uid="{0141266D-28EC-E044-97D4-AA3617150640}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0141266D-28EC-E044-97D4-AA3617150640}" name="Tableau36" displayName="Tableau36" ref="C24:D34" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="C24:D34" xr:uid="{0141266D-28EC-E044-97D4-AA3617150640}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{80CEAE2F-D404-0343-A508-5DE933EAB6B8}" name="ID" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{76112267-6DFB-124A-8252-98AA691C1E0A}" name="Process"/>
@@ -427,10 +427,10 @@
   <autoFilter ref="A4:E16" xr:uid="{780F29F6-8EB6-1C49-BE5B-5D3BD5DAA6CC}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C7FBFF3B-8D2E-914E-B3AB-30042E858C41}" name="Entity-user matrix"/>
-    <tableColumn id="2" xr3:uid="{80BABC81-F535-944D-B923-AF76A05ADEDF}" name="customer"/>
-    <tableColumn id="3" xr3:uid="{04F1F718-C205-0D49-B6DF-E17E70E0A5BD}" name="employee"/>
-    <tableColumn id="4" xr3:uid="{67ECC177-4807-7D43-948B-010EDB4A692C}" name="admin app"/>
+    <tableColumn id="3" xr3:uid="{04F1F718-C205-0D49-B6DF-E17E70E0A5BD}" name="Employee"/>
+    <tableColumn id="4" xr3:uid="{67ECC177-4807-7D43-948B-010EDB4A692C}" name="Admin app"/>
     <tableColumn id="16" xr3:uid="{4E8DADAC-5239-144A-A73F-69D51FE53FBF}" name="Fleet responsible"/>
+    <tableColumn id="5" xr3:uid="{FEDF6E9F-2A5A-422A-803A-B6D5C4C3627D}" name="HR manager"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -733,16 +733,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F84E62-A628-A646-8A10-5F57E6471DE6}">
-  <dimension ref="B3:L29"/>
+  <dimension ref="B3:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="28.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.58203125" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -752,180 +752,196 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
       <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>15</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>16</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:12">
       <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:12">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:12">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12">
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:12">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
+    <row r="15" spans="2:12">
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
       <c r="B21" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
       <c r="B22" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
       <c r="B23" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
       <c r="B24" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
       <c r="B25" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3">
-      <c r="B28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -940,15 +956,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B62E4D6-429A-A64E-80AA-0D0F39004CC0}">
-  <dimension ref="B4:O35"/>
+  <dimension ref="B4:O34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <cols>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.9140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
@@ -957,245 +973,221 @@
   <sheetData>
     <row r="4" spans="2:15" ht="23">
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
       <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" t="s">
         <v>14</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>15</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>16</v>
-      </c>
-      <c r="K4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:15">
       <c r="B5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
       </c>
       <c r="J5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="L5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:15">
       <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="L6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="25">
       <c r="B7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="L7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:15">
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="L8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="2:15">
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="2:15">
       <c r="B10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="K10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:15">
       <c r="B11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:15">
       <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="2:15">
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="K13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:15">
       <c r="B14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="2:15">
       <c r="B15" t="s">
-        <v>2</v>
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
       </c>
       <c r="H15" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="I15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="2:15">
       <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4">
+      <c r="C24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4">
+      <c r="C25" t="s">
         <v>3</v>
       </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" t="s">
-        <v>43</v>
-      </c>
-      <c r="I16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12">
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" t="s">
-        <v>43</v>
-      </c>
-      <c r="L17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12">
-      <c r="C25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12">
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4">
       <c r="C26" t="s">
         <v>4</v>
       </c>
@@ -1203,7 +1195,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="2:12">
+    <row r="27" spans="3:4">
       <c r="C27" t="s">
         <v>5</v>
       </c>
@@ -1211,68 +1203,60 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="2:12">
+    <row r="28" spans="3:4">
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4">
       <c r="C29" t="s">
         <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="2:12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4">
       <c r="C30" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4">
+      <c r="C31" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="2:12">
-      <c r="C31" t="s">
+      <c r="D31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4">
+      <c r="C32" t="s">
         <v>14</v>
       </c>
-      <c r="D31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12">
-      <c r="C32" t="s">
-        <v>15</v>
-      </c>
       <c r="D32" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="3:4">
       <c r="C33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="3:4">
       <c r="C34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4">
-      <c r="C35" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1287,16 +1271,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{138BF9B9-C166-BA41-94A8-F1764334ED68}">
-  <dimension ref="A4:E16"/>
+  <dimension ref="A4:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
@@ -1307,155 +1291,147 @@
   <sheetData>
     <row r="4" spans="1:5" ht="23">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>50</v>
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>50</v>
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" t="s">
-        <v>50</v>
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>50</v>
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>52</v>
       </c>
-      <c r="C10" t="s">
-        <v>44</v>
+      <c r="D10" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>53</v>
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>50</v>
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:passport_control: finish privilege and role file
</commit_message>
<xml_diff>
--- a/Matrix.xlsx
+++ b/Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\DataGripProjects\db-security-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44633F7-3100-4D8D-9EB2-37D5ADB9D75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B26B0A7-7C12-4C29-BFEC-F28B0E02DD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{FB151949-07DF-9E4B-ADDA-32C56BC4D90F}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="2" xr2:uid="{FB151949-07DF-9E4B-ADDA-32C56BC4D90F}"/>
   </bookViews>
   <sheets>
     <sheet name="Process-user matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="59">
   <si>
     <t>Process-user matrix</t>
   </si>
@@ -209,6 +209,12 @@
   </si>
   <si>
     <t>Admin can also manage the list of states</t>
+  </si>
+  <si>
+    <t>I,U,D,S</t>
+  </si>
+  <si>
+    <t>I,U</t>
   </si>
 </sst>
 </file>
@@ -736,7 +742,7 @@
   <dimension ref="B3:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -959,7 +965,7 @@
   <dimension ref="B4:O34"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -967,7 +973,10 @@
     <col min="2" max="2" width="33.9140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.9140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="76.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1023,7 +1032,7 @@
         <v>39</v>
       </c>
       <c r="L5" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:15">
@@ -1042,7 +1051,7 @@
         <v>39</v>
       </c>
       <c r="L7" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>23</v>
@@ -1059,7 +1068,7 @@
         <v>39</v>
       </c>
       <c r="L8" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="2:15">
@@ -1073,7 +1082,7 @@
         <v>39</v>
       </c>
       <c r="L9" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:15">
@@ -1101,7 +1110,7 @@
         <v>35</v>
       </c>
       <c r="H11" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="2:15">
@@ -1112,7 +1121,7 @@
         <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="G12" t="s">
         <v>39</v>
@@ -1151,10 +1160,10 @@
         <v>39</v>
       </c>
       <c r="H15" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="I15" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="2:15">
@@ -1168,7 +1177,7 @@
         <v>39</v>
       </c>
       <c r="I16" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="3:4">
@@ -1274,7 +1283,7 @@
   <dimension ref="A4:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
@@ -1314,7 +1323,7 @@
         <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1333,7 +1342,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1341,7 +1350,7 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1352,7 +1361,7 @@
         <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1371,7 +1380,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1379,7 +1388,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -1407,7 +1416,7 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1418,10 +1427,10 @@
         <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:2">

</xml_diff>

<commit_message>
:memo: just saving my work in case of shit happens
</commit_message>
<xml_diff>
--- a/Matrix.xlsx
+++ b/Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\DataGripProjects\db-security-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B26B0A7-7C12-4C29-BFEC-F28B0E02DD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00FED28-D116-4BD9-A605-C18B2E0928A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="2" xr2:uid="{FB151949-07DF-9E4B-ADDA-32C56BC4D90F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB151949-07DF-9E4B-ADDA-32C56BC4D90F}"/>
   </bookViews>
   <sheets>
     <sheet name="Process-user matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="59">
   <si>
     <t>Process-user matrix</t>
   </si>
@@ -187,9 +187,6 @@
     <t>Manage employees</t>
   </si>
   <si>
-    <t>The fleet responsible use a procedure to cancel a vehicle reservation if he put a vehicle as damaged</t>
-  </si>
-  <si>
     <t>For scalability reason customers are users at application level</t>
   </si>
   <si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>I,U</t>
+  </si>
+  <si>
+    <t>Employees need this permission in order to call the procedure used to change a vehicule state</t>
   </si>
 </sst>
 </file>
@@ -741,19 +741,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F84E62-A628-A646-8A10-5F57E6471DE6}">
   <dimension ref="B3:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="33.58203125" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.625" customWidth="1"/>
+    <col min="3" max="3" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="5.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="23">
+    <row r="3" spans="2:12" ht="23.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -812,6 +812,9 @@
       <c r="K5" t="s">
         <v>19</v>
       </c>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="2:12">
       <c r="B6" t="s">
@@ -845,9 +848,6 @@
       <c r="B8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
       <c r="L8" t="s">
         <v>19</v>
       </c>
@@ -872,7 +872,7 @@
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:5">
@@ -882,9 +882,6 @@
       <c r="C17" t="s">
         <v>9</v>
       </c>
-      <c r="E17" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" t="s">
@@ -948,6 +945,9 @@
       </c>
       <c r="C25" t="s">
         <v>37</v>
+      </c>
+      <c r="E25" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -964,23 +964,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B62E4D6-429A-A64E-80AA-0D0F39004CC0}">
   <dimension ref="B4:O34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="33.9140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="4.9140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="76.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="33.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="42.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="76.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:15" ht="23">
+    <row r="4" spans="2:15" ht="23.25">
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>39</v>
       </c>
       <c r="L5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="2:15">
@@ -1043,7 +1043,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="25">
+    <row r="7" spans="2:15" ht="25.5">
       <c r="B7" t="s">
         <v>26</v>
       </c>
@@ -1051,11 +1051,9 @@
         <v>39</v>
       </c>
       <c r="L7" t="s">
-        <v>57</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="O7" s="3"/>
     </row>
     <row r="8" spans="2:15">
       <c r="B8" t="s">
@@ -1068,7 +1066,7 @@
         <v>39</v>
       </c>
       <c r="L8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:15">
@@ -1082,7 +1080,7 @@
         <v>39</v>
       </c>
       <c r="L9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="2:15">
@@ -1093,7 +1091,7 @@
         <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s">
         <v>39</v>
@@ -1110,7 +1108,7 @@
         <v>35</v>
       </c>
       <c r="H11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="2:15">
@@ -1121,7 +1119,7 @@
         <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G12" t="s">
         <v>39</v>
@@ -1151,7 +1149,7 @@
     </row>
     <row r="15" spans="2:15">
       <c r="B15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
         <v>39</v>
@@ -1160,10 +1158,10 @@
         <v>39</v>
       </c>
       <c r="H15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="2:15">
@@ -1177,18 +1175,21 @@
         <v>39</v>
       </c>
       <c r="I16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13">
       <c r="C24" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="3:4">
+      <c r="M24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13">
       <c r="C25" t="s">
         <v>3</v>
       </c>
@@ -1196,7 +1197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="3:4">
+    <row r="26" spans="3:13">
       <c r="C26" t="s">
         <v>4</v>
       </c>
@@ -1204,7 +1205,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="3:4">
+    <row r="27" spans="3:13">
       <c r="C27" t="s">
         <v>5</v>
       </c>
@@ -1212,7 +1213,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="3:4">
+    <row r="28" spans="3:13">
       <c r="C28" t="s">
         <v>6</v>
       </c>
@@ -1220,7 +1221,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="3:4">
+    <row r="29" spans="3:13">
       <c r="C29" t="s">
         <v>7</v>
       </c>
@@ -1228,7 +1229,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="3:4">
+    <row r="30" spans="3:13">
       <c r="C30" t="s">
         <v>12</v>
       </c>
@@ -1236,7 +1237,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="3:4">
+    <row r="31" spans="3:13">
       <c r="C31" t="s">
         <v>13</v>
       </c>
@@ -1244,7 +1245,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="3:4">
+    <row r="32" spans="3:13">
       <c r="C32" t="s">
         <v>14</v>
       </c>
@@ -1282,23 +1283,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{138BF9B9-C166-BA41-94A8-F1764334ED68}">
   <dimension ref="A4:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="76.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="76.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" ht="23">
+    <row r="4" spans="1:5" ht="23.25">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -1306,7 +1307,7 @@
         <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
         <v>43</v>
@@ -1320,16 +1321,19 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>25</v>
       </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
       <c r="C6" t="s">
         <v>38</v>
       </c>
@@ -1342,7 +1346,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1350,7 +1354,7 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1361,7 +1365,7 @@
         <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1369,10 +1373,10 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1380,7 +1384,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1388,7 +1392,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -1405,7 +1409,7 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1416,31 +1420,31 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
         <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(audit): fix first part of audit script
</commit_message>
<xml_diff>
--- a/Matrix.xlsx
+++ b/Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\DataGripProjects\db-security-2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Vanhaeren\DataGripProjects\dbsec\db-security-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00FED28-D116-4BD9-A605-C18B2E0928A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F06203-3282-4C53-8193-6F7EC047C181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB151949-07DF-9E4B-ADDA-32C56BC4D90F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{FB151949-07DF-9E4B-ADDA-32C56BC4D90F}"/>
   </bookViews>
   <sheets>
     <sheet name="Process-user matrix" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="64">
   <si>
     <t>Process-user matrix</t>
   </si>
@@ -202,9 +202,6 @@
     <t>Admin app</t>
   </si>
   <si>
-    <t>S,I</t>
-  </si>
-  <si>
     <t>Admin can also manage the list of states</t>
   </si>
   <si>
@@ -215,6 +212,24 @@
   </si>
   <si>
     <t>Employees need this permission in order to call the procedure used to change a vehicule state</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>Manage Check-in</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>Manage Returns</t>
+  </si>
+  <si>
+    <t>U,D</t>
+  </si>
+  <si>
+    <t>S,I,U,D</t>
   </si>
 </sst>
 </file>
@@ -271,11 +286,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,9 +383,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD3C6F1B-018A-814A-BAB2-8F3FAE647CD3}" name="Tableau1" displayName="Tableau1" ref="B3:L8" totalsRowShown="0">
-  <autoFilter ref="B3:L8" xr:uid="{AD3C6F1B-018A-814A-BAB2-8F3FAE647CD3}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD3C6F1B-018A-814A-BAB2-8F3FAE647CD3}" name="Tableau1" displayName="Tableau1" ref="B3:N8" totalsRowShown="0">
+  <autoFilter ref="B3:N8" xr:uid="{AD3C6F1B-018A-814A-BAB2-8F3FAE647CD3}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{6E0619E5-D273-D74D-AF9D-840719E1F688}" name="Process-user matrix"/>
     <tableColumn id="2" xr3:uid="{73682482-EF9F-2B41-B13A-604249596F4B}" name="P1"/>
     <tableColumn id="3" xr3:uid="{D39BF275-0D49-F349-B278-9A09A60704CB}" name="P2"/>
@@ -381,14 +397,16 @@
     <tableColumn id="9" xr3:uid="{6825D153-7B92-AC4D-BA31-10A5A3FE04DE}" name="P8"/>
     <tableColumn id="10" xr3:uid="{2D051CD8-7624-754B-8CB1-82EA6944B53D}" name="P9"/>
     <tableColumn id="12" xr3:uid="{737D8829-17F6-2942-82FC-C05DA9C7D4AB}" name="P10"/>
+    <tableColumn id="11" xr3:uid="{FBC828E3-F337-4899-A224-51D5705222BC}" name="P11"/>
+    <tableColumn id="13" xr3:uid="{DFEAE47A-174E-4CA2-9B99-79F891DE3B5C}" name="P12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{285ED5D0-9C49-48D1-B580-D390634D232F}" name="Tableau363" displayName="Tableau363" ref="B15:C25" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="B15:C25" xr:uid="{285ED5D0-9C49-48D1-B580-D390634D232F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{285ED5D0-9C49-48D1-B580-D390634D232F}" name="Tableau363" displayName="Tableau363" ref="B15:C27" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="B15:C27" xr:uid="{285ED5D0-9C49-48D1-B580-D390634D232F}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{35459B5A-4B3E-4530-8321-9B450516126A}" name="ID" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{A5DE6B87-05C4-4E7F-8554-0EB8B0B8AB38}" name="Process"/>
@@ -398,9 +416,9 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B43A4B11-A654-8342-87E0-FF434B9827DC}" name="Tableau15" displayName="Tableau15" ref="B4:L16" totalsRowShown="0">
-  <autoFilter ref="B4:L16" xr:uid="{B43A4B11-A654-8342-87E0-FF434B9827DC}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B43A4B11-A654-8342-87E0-FF434B9827DC}" name="Tableau15" displayName="Tableau15" ref="B4:N16" totalsRowShown="0">
+  <autoFilter ref="B4:N16" xr:uid="{B43A4B11-A654-8342-87E0-FF434B9827DC}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{4FAFE25D-D33B-BB45-B051-60611B74A325}" name="Entity-process matrix"/>
     <tableColumn id="2" xr3:uid="{B43170F5-2DC5-AD4D-8F11-C5EDFA8381E4}" name="P1"/>
     <tableColumn id="3" xr3:uid="{72D0B51C-A9FC-7B46-BFA3-ADFA50A19FB0}" name="P2"/>
@@ -412,14 +430,16 @@
     <tableColumn id="9" xr3:uid="{1CF34A13-89C0-2B43-B926-615A5AA68652}" name="P8"/>
     <tableColumn id="10" xr3:uid="{33CA9CCF-C943-574E-9868-B38F0C4EB750}" name="P9"/>
     <tableColumn id="12" xr3:uid="{64C573FF-A395-DD40-AD2C-33100D180B3E}" name="P10"/>
+    <tableColumn id="11" xr3:uid="{E1AB0558-8475-4BA5-B614-26BD0CE31BAC}" name="P11"/>
+    <tableColumn id="13" xr3:uid="{4D212AEA-C2E8-4F1C-9938-FF9CD7CBECB8}" name="P12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0141266D-28EC-E044-97D4-AA3617150640}" name="Tableau36" displayName="Tableau36" ref="C24:D34" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="C24:D34" xr:uid="{0141266D-28EC-E044-97D4-AA3617150640}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0141266D-28EC-E044-97D4-AA3617150640}" name="Tableau36" displayName="Tableau36" ref="B20:C32" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="B20:C32" xr:uid="{0141266D-28EC-E044-97D4-AA3617150640}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{80CEAE2F-D404-0343-A508-5DE933EAB6B8}" name="ID" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{76112267-6DFB-124A-8252-98AA691C1E0A}" name="Process"/>
@@ -443,9 +463,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -483,7 +503,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -589,7 +609,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -731,7 +751,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -739,21 +759,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F84E62-A628-A646-8A10-5F57E6471DE6}">
-  <dimension ref="B3:L25"/>
+  <dimension ref="B3:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="33.625" customWidth="1"/>
-    <col min="3" max="3" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.59765625" customWidth="1"/>
+    <col min="3" max="3" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" ht="23.25">
+    <row r="3" spans="2:14" ht="22.8">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -787,8 +808,14 @@
       <c r="L3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="2:12">
+      <c r="M3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
       <c r="B4" t="s">
         <v>47</v>
       </c>
@@ -796,7 +823,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:14">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -815,8 +842,14 @@
       <c r="L5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="2:12">
+      <c r="M5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -836,7 +869,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:14">
       <c r="B7" t="s">
         <v>45</v>
       </c>
@@ -844,7 +877,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:14">
       <c r="B8" t="s">
         <v>46</v>
       </c>
@@ -852,11 +885,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="2:14">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:14">
       <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
@@ -864,7 +897,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="2:14">
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -947,7 +980,23 @@
         <v>37</v>
       </c>
       <c r="E25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="4" t="s">
         <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -962,25 +1011,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B62E4D6-429A-A64E-80AA-0D0F39004CC0}">
-  <dimension ref="B4:O34"/>
+  <dimension ref="B4:O32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="3" width="33.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="42.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="76.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="33.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="6.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="76.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:15" ht="23.25">
+    <row r="4" spans="2:15" ht="22.8">
       <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1013,6 +1062,12 @@
       </c>
       <c r="L4" t="s">
         <v>16</v>
+      </c>
+      <c r="M4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:15">
@@ -1032,7 +1087,7 @@
         <v>39</v>
       </c>
       <c r="L5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:15">
@@ -1043,7 +1098,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="25.5">
+    <row r="7" spans="2:15" ht="24.6">
       <c r="B7" t="s">
         <v>26</v>
       </c>
@@ -1051,7 +1106,7 @@
         <v>39</v>
       </c>
       <c r="L7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O7" s="3"/>
     </row>
@@ -1066,7 +1121,7 @@
         <v>39</v>
       </c>
       <c r="L8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="2:15">
@@ -1080,7 +1135,7 @@
         <v>39</v>
       </c>
       <c r="L9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:15">
@@ -1108,7 +1163,7 @@
         <v>35</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:15">
@@ -1119,7 +1174,7 @@
         <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s">
         <v>39</v>
@@ -1135,6 +1190,9 @@
       <c r="K13" t="s">
         <v>36</v>
       </c>
+      <c r="M13" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="14" spans="2:15">
       <c r="B14" t="s">
@@ -1146,6 +1204,9 @@
       <c r="J14" t="s">
         <v>36</v>
       </c>
+      <c r="N14" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="15" spans="2:15">
       <c r="B15" t="s">
@@ -1158,10 +1219,10 @@
         <v>39</v>
       </c>
       <c r="H15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="2:15">
@@ -1175,98 +1236,116 @@
         <v>39</v>
       </c>
       <c r="I16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="3:13">
-      <c r="C24" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="3:13">
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
       <c r="C25" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="3:13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
       <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="3:13">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
       <c r="C27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="3:13">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
       <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="3:13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
       <c r="C29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="3:13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
       <c r="C30" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="3:13">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="C31" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="3:13">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="C32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4">
-      <c r="C33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4">
-      <c r="C34" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1283,23 +1362,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{138BF9B9-C166-BA41-94A8-F1764334ED68}">
   <dimension ref="A4:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="76.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="76.09765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" ht="23.25">
+    <row r="4" spans="1:5" ht="22.8">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -1324,7 +1403,7 @@
         <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1346,7 +1425,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1354,7 +1433,7 @@
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1365,7 +1444,7 @@
         <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1384,7 +1463,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1392,7 +1471,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -1401,7 +1480,7 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1409,7 +1488,7 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1420,7 +1499,7 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1431,10 +1510,10 @@
         <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="2:2">
@@ -1444,7 +1523,7 @@
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>